<commit_message>
change done for admin pannel
</commit_message>
<xml_diff>
--- a/product.xlsx
+++ b/product.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BookMartBackEnd\BookMartBackEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5139C2-8A3A-4663-A0B2-468E00C01703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E24AAD-A9F8-4A73-B168-DA57C51B069E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C0BCD9F3-841E-4B2A-AF2D-D3EC60A4B537}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>productName</t>
   </si>
@@ -42,12 +42,6 @@
     <t>isActive</t>
   </si>
   <si>
-    <t>Rich Dad Poor Dad</t>
-  </si>
-  <si>
-    <t>image url</t>
-  </si>
-  <si>
     <t>this is book</t>
   </si>
   <si>
@@ -57,7 +51,25 @@
     <t>subCategory</t>
   </si>
   <si>
+    <t>Gunhoa ka devta</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1357204311i/6720421.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1517755071i/3282557.jpg</t>
+  </si>
+  <si>
+    <t>suraj ka satva ghoda</t>
+  </si>
+  <si>
     <t>law Book</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Hindi</t>
   </si>
   <si>
     <t>English</t>
@@ -67,10 +79,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,13 +113,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,16 +435,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406BC9E3-CF85-445C-83C8-E9D3DA5A1A24}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" customWidth="1"/>
     <col min="4" max="4" width="18.81640625" customWidth="1"/>
     <col min="5" max="5" width="13.36328125" customWidth="1"/>
@@ -440,10 +463,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -454,28 +477,54 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C2">
         <v>234</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>455</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{AFBBA43C-68F9-4129-BB3D-D865B89937CF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>